<commit_message>
[PHOENIX-6061] test data changed for PGR as per new dump
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="124">
   <si>
     <t>dataName</t>
   </si>
@@ -197,9 +197,6 @@
     <t>LightingSuperintendent</t>
   </si>
   <si>
-    <t>Ceelam Ramesh Babu</t>
-  </si>
-  <si>
     <t>Sanctioned and shall grievance be processed</t>
   </si>
   <si>
@@ -390,6 +387,12 @@
   </si>
   <si>
     <t>Chandragiri Murali Krishna ~ PHS_Sanitary Inspector_6</t>
+  </si>
+  <si>
+    <t>RAVI BABU GUNDAM PATI</t>
+  </si>
+  <si>
+    <t>Veterinary officer</t>
   </si>
 </sst>
 </file>
@@ -762,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1040,36 +1043,36 @@
         <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>26</v>
@@ -1086,7 +1089,7 @@
     </row>
     <row r="19" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>26</v>
@@ -1103,7 +1106,7 @@
     </row>
     <row r="20" spans="1:6" ht="31.35" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>26</v>
@@ -1112,7 +1115,7 @@
         <v>46</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>48</v>
@@ -1120,38 +1123,38 @@
     </row>
     <row r="21" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -1160,7 +1163,7 @@
         <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>9</v>
@@ -1168,7 +1171,7 @@
     </row>
     <row r="24" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -1177,15 +1180,15 @@
         <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -1194,7 +1197,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>17</v>
@@ -1202,133 +1205,133 @@
     </row>
     <row r="26" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A29" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A31" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="17.850000000000001" customHeight="1">
       <c r="A33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="17.850000000000001" customHeight="1">
       <c r="A34" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="17.850000000000001" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>6</v>
@@ -1337,12 +1340,12 @@
         <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="17.850000000000001" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>19</v>
@@ -1351,12 +1354,12 @@
         <v>20</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>19</v>
@@ -1365,7 +1368,7 @@
         <v>20</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>22</v>
@@ -1373,7 +1376,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>50</v>
@@ -1382,15 +1385,15 @@
         <v>51</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>6</v>
@@ -1407,7 +1410,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>6</v>
@@ -1424,7 +1427,7 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>6</v>
@@ -1441,7 +1444,7 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>19</v>
@@ -1450,7 +1453,7 @@
         <v>20</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX-7825] modified the changes in tax exemption and approval details
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="150">
   <si>
     <t xml:space="preserve">dataName</t>
   </si>
@@ -448,6 +448,30 @@
   </si>
   <si>
     <t xml:space="preserve">PTCommissionerOne ~ ADM_COMM_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTISBillCollector1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTBillCollectorOne~PTIS_REVBC_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTISRevenueInspector1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTRevenueInspectorOne~PTIS_REVSI_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTISRevenueOfficer1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTRevenueOfficerOne~PTIS_REVOF_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTISCommissioner1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PTCommissionerOne~ADM_COMM_20</t>
   </si>
 </sst>
 </file>
@@ -509,8 +533,9 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Ubuntu"/>
-      <family val="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -559,7 +584,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -581,10 +606,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -610,21 +631,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A32" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B56" activeCellId="0" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.5102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.4285714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="55.4795918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.4540816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.0255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="54.8061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.0459183673469"/>
     <col collapsed="false" hidden="false" max="257" min="6" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1344,7 +1365,7 @@
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -1397,6 +1418,71 @@
       </c>
       <c r="D46" s="1" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1422,6 +1508,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1445,6 +1534,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
[PHOENIX-5854] - Manual Test Cases that was in eGov-QA repository
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
@@ -188,9 +188,6 @@
     <t>sanitaryInspector1</t>
   </si>
   <si>
-    <t>TLSanitoryInspectorOne</t>
-  </si>
-  <si>
     <t>Funds needed to resolve the issue</t>
   </si>
   <si>
@@ -504,6 +501,9 @@
   </si>
   <si>
     <t>TLSanitarySupervisorOne~TL_SS_01</t>
+  </si>
+  <si>
+    <t>TLSanitoryInspectorOne [TL_SI_01]</t>
   </si>
 </sst>
 </file>
@@ -883,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1161,52 +1161,52 @@
         <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="F15"/>
     </row>
     <row r="16" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="F16"/>
     </row>
     <row r="17" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>26</v>
@@ -1223,7 +1223,7 @@
     </row>
     <row r="19" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>26</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="20" spans="1:6" ht="31.35" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>26</v>
@@ -1249,7 +1249,7 @@
         <v>46</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>48</v>
@@ -1257,39 +1257,39 @@
     </row>
     <row r="21" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="E22"/>
     </row>
     <row r="23" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -1298,7 +1298,7 @@
         <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>9</v>
@@ -1306,7 +1306,7 @@
     </row>
     <row r="24" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -1315,15 +1315,15 @@
         <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -1332,7 +1332,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>17</v>
@@ -1340,142 +1340,142 @@
     </row>
     <row r="26" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="E26"/>
     </row>
     <row r="27" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A27" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="E27"/>
     </row>
     <row r="28" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A29" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="E29"/>
     </row>
     <row r="30" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="D30" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="E30"/>
     </row>
     <row r="31" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="E31"/>
     </row>
     <row r="32" spans="1:6" ht="17.850000000000001" customHeight="1">
       <c r="A32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="E32"/>
     </row>
     <row r="33" spans="1:5" ht="17.850000000000001" customHeight="1">
       <c r="A33" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="E33"/>
     </row>
     <row r="34" spans="1:5" ht="17.850000000000001" customHeight="1">
       <c r="A34" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C34" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="E34"/>
     </row>
     <row r="35" spans="1:5" ht="17.850000000000001" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>6</v>
@@ -1484,13 +1484,13 @@
         <v>15</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E35"/>
     </row>
     <row r="36" spans="1:5" ht="17.850000000000001" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>19</v>
@@ -1499,13 +1499,13 @@
         <v>20</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E36"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>19</v>
@@ -1514,7 +1514,7 @@
         <v>20</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>22</v>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>50</v>
@@ -1531,83 +1531,83 @@
         <v>51</v>
       </c>
       <c r="D38" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="E40" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="E41" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>6</v>
@@ -1616,7 +1616,7 @@
         <v>7</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>9</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>6</v>
@@ -1633,7 +1633,7 @@
         <v>11</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>13</v>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>6</v>
@@ -1650,7 +1650,7 @@
         <v>15</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>17</v>
@@ -1658,7 +1658,7 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>19</v>
@@ -1667,12 +1667,12 @@
         <v>20</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>6</v>
@@ -1681,7 +1681,7 @@
         <v>7</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>9</v>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>6</v>
@@ -1698,7 +1698,7 @@
         <v>11</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>13</v>
@@ -1706,7 +1706,7 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>6</v>
@@ -1715,7 +1715,7 @@
         <v>15</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>17</v>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>19</v>
@@ -1732,12 +1732,12 @@
         <v>20</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>19</v>
@@ -1746,7 +1746,7 @@
         <v>20</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>22</v>
@@ -1754,7 +1754,7 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>50</v>
@@ -1763,78 +1763,78 @@
         <v>51</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PHOENIX - 5854] test data change and minor workflow fix for TL automation
</commit_message>
<xml_diff>
--- a/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
+++ b/egov/egov_functional_test/src/test/resources/dataFiles/approvalDetailsTestData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="162">
   <si>
     <t>dataName</t>
   </si>
@@ -488,22 +488,25 @@
     <t>TL_SS1</t>
   </si>
   <si>
-    <t>TLSanitoryInspectorOne~TL_SI_01</t>
-  </si>
-  <si>
-    <t>TLAMOHOne~TL_AMOH_10</t>
-  </si>
-  <si>
-    <t>TLMHO~TL_MHO_01</t>
-  </si>
-  <si>
-    <t>TLCMOH~TL_CMOH_01</t>
-  </si>
-  <si>
-    <t>TLSanitarySupervisorOne~TL_SS_01</t>
-  </si>
-  <si>
     <t>TLSanitoryInspectorOne [TL_SI_01]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLSanitoryInspectorOne [TL_SI_01] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLAMOHOne [TL_AMOH_10] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLMHO [TL_MHO_01] </t>
+  </si>
+  <si>
+    <t>TLCMOH [TL_CMOH_01]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLSanitarySupervisorOne [TL_SS_01] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TLCommissionerOne [ADM_COMM_1] </t>
   </si>
 </sst>
 </file>
@@ -883,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1161,7 +1164,7 @@
         <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>55</v>
@@ -1746,7 +1749,7 @@
         <v>20</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>115</v>
+        <v>161</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>22</v>
@@ -1763,7 +1766,7 @@
         <v>51</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>118</v>
@@ -1780,7 +1783,7 @@
         <v>120</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>122</v>
@@ -1797,7 +1800,7 @@
         <v>124</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>122</v>
@@ -1814,7 +1817,7 @@
         <v>127</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>122</v>
@@ -1831,7 +1834,7 @@
         <v>130</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>132</v>

</xml_diff>